<commit_message>
add game Tresure hunt
</commit_message>
<xml_diff>
--- a/100 projects_list.xlsx
+++ b/100 projects_list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3951E45A-B179-4E89-AD92-94FD07435B4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526BCE31-CA36-436E-BD68-FC029CAC9525}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>DAY1</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>Tip _calculator</t>
+  </si>
+  <si>
+    <t>Conditional Statements,Logical Operators,Code Blocks and Scope</t>
+  </si>
+  <si>
+    <t>Find_Tresure</t>
   </si>
 </sst>
 </file>
@@ -652,7 +658,7 @@
   <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,6 +693,12 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">

</xml_diff>